<commit_message>
changed splitters on refineries to delimiters on options
</commit_message>
<xml_diff>
--- a/records_maps/Capstone Maps/abcnorio-map2019.xlsx
+++ b/records_maps/Capstone Maps/abcnorio-map2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jfreedma/Documents/GitHub/zinecat.org/records_maps/Capstone Maps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BFB82D-6CEE-DF41-9E5F-1C7B4C8FB509}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC3385A-59F9-8A46-8C24-A7DC0FED5FDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2240" yWindow="520" windowWidth="24500" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="100">
   <si>
     <t>Mapping</t>
   </si>
@@ -333,9 +333,6 @@
   </si>
   <si>
     <t>{ "relationshipType": "part_of", "collectionType": "external" }</t>
-  </si>
-  <si>
-    <t>{"delimiter": ",", "relationshipType": "is described by", "list": "zinecatsubject"}</t>
   </si>
   <si>
     <t>{"delimiter": ",","list": "languages"}</t>
@@ -786,8 +783,8 @@
   <dimension ref="A1:Z1017"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="137" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="16"/>
@@ -940,7 +937,9 @@
         <v>84</v>
       </c>
       <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+      <c r="E4" s="10" t="s">
+        <v>96</v>
+      </c>
       <c r="F4" s="13"/>
       <c r="G4" s="4"/>
       <c r="H4" s="7"/>
@@ -1233,12 +1232,14 @@
       <c r="C13" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E13" s="10"/>
+      <c r="E13" s="10" t="s">
+        <v>96</v>
+      </c>
       <c r="F13" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
@@ -1276,7 +1277,7 @@
         <v>88</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
@@ -1568,7 +1569,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>

</xml_diff>